<commit_message>
Fix template spelling, dicipline -> discipline in vars_meta_data.
</commit_message>
<xml_diff>
--- a/template/datasetTemplate.xlsx
+++ b/template/datasetTemplate.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FA4FD84-2114-BF4C-A080-BA134A3897AA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -161,12 +162,6 @@
     <t>&lt; placeholder for missing values (examples: empty cell, "nan", "unknown", #FFFF) &gt;  ↓</t>
   </si>
   <si>
-    <t>var_dicipline</t>
-  </si>
-  <si>
-    <t>&lt; associated diciple(s) (&lt;100 chars) (examples: [Physics, Chemistry, Biology, BioGeoChemistry, etc..] )&gt;  ↓</t>
-  </si>
-  <si>
     <t>dataset_history</t>
   </si>
   <si>
@@ -207,12 +202,18 @@
   </si>
   <si>
     <t>https://zenodo.org/</t>
+  </si>
+  <si>
+    <t>var_discipline</t>
+  </si>
+  <si>
+    <t>&lt; associated discipline(s) (&lt;100 chars) (examples: [Physics, Chemistry, Biology, BioGeoChemistry, etc..] )&gt;  ↓</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -553,25 +554,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="77.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="72.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="74.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="14.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="2"/>
+    <col min="8" max="8" width="15.5" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -620,7 +621,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
     </row>
   </sheetData>
@@ -630,26 +631,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46" style="2" customWidth="1"/>
-    <col min="2" max="4" width="46.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="82.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="58.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="46.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="51.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="4" width="46.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="82.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="47.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="58.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="53.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="46.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="51.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="37.1640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -663,16 +664,16 @@
         <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
@@ -681,7 +682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -689,22 +690,22 @@
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>19</v>
@@ -713,54 +714,56 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G3" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G5" s="3" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G5" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="83.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="100.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="81.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="67.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="81.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="98.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="49.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="41.140625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="41.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="83.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="100.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="81.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="67.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="81.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="98.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="49.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="41.1640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -771,7 +774,7 @@
         <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>24</v>
@@ -786,7 +789,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>41</v>
@@ -795,7 +798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -806,7 +809,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>30</v>
@@ -821,7 +824,7 @@
         <v>45</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>42</v>
@@ -830,22 +833,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>

</xml_diff>